<commit_message>
Added pH Box Plot
</commit_message>
<xml_diff>
--- a/Prototype Programs/Protoype Sensors/Colour Sensor/ColourSensorDatabase (version 1).xlsx
+++ b/Prototype Programs/Protoype Sensors/Colour Sensor/ColourSensorDatabase (version 1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UTS\Autumn 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C522A076-2864-4A37-84BB-7D9921B012D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CA8414-3843-4F54-90B9-5181CA8C6A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coke Colour" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,22 @@
     <sheet name="Beer pH" sheetId="4" r:id="rId7"/>
     <sheet name="Coffee pH" sheetId="6" r:id="rId8"/>
     <sheet name="Tea pH" sheetId="8" r:id="rId9"/>
+    <sheet name="pH Box Plot" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Coke Colour'!$A$1:$K$17</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">'Colour Box Plot'!$G$2:$G$6</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Colour Box Plot'!$G$2:$G$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Colour Box Plot'!$H$2:$H$6</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Colour Box Plot'!$I$2:$I$6</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Colour Box Plot'!$J$2:$J$6</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Colour Box Plot'!$H$2:$H$6</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'pH Box Plot'!$I$2:$I$6</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'pH Box Plot'!$J$2:$J$6</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Colour Box Plot'!$I$2:$I$6</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Colour Box Plot'!$J$2:$J$6</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'pH Box Plot'!$G$2:$G$6</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'pH Box Plot'!$H$2:$H$6</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'pH Box Plot'!$I$2:$I$6</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'pH Box Plot'!$J$2:$J$6</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'pH Box Plot'!$G$2:$G$6</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'pH Box Plot'!$H$2:$H$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -53,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="27">
   <si>
     <t>Red</t>
   </si>
@@ -123,6 +131,18 @@
   <si>
     <t>Max</t>
   </si>
+  <si>
+    <t>Coke</t>
+  </si>
+  <si>
+    <t>Beer</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Tea</t>
+  </si>
 </sst>
 </file>
 
@@ -181,22 +201,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -237,6 +257,9 @@
               <cx:v>Coke</cx:v>
             </cx:txData>
           </cx:tx>
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
@@ -249,6 +272,9 @@
               <cx:v>Beer</cx:v>
             </cx:txData>
           </cx:tx>
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
           <cx:dataId val="1"/>
           <cx:layoutPr>
             <cx:statistics quartileMethod="exclusive"/>
@@ -260,6 +286,27 @@
               <cx:v>Coffee</cx:v>
             </cx:txData>
           </cx:tx>
+          <cx:dataLabels>
+            <cx:txPr>
+              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:endParaRPr>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
           <cx:dataId val="2"/>
           <cx:layoutPr>
             <cx:statistics quartileMethod="exclusive"/>
@@ -271,6 +318,9 @@
               <cx:v>Tea</cx:v>
             </cx:txData>
           </cx:tx>
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
           <cx:dataId val="3"/>
           <cx:layoutPr>
             <cx:statistics quartileMethod="exclusive"/>
@@ -322,7 +372,213 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.10</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.11</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>pH Paper Hue Values</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>pH Paper Hue Values</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{8CCA57B9-44D7-48FB-B381-CC70CBCFDE6E}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Coke</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{241C5B70-4B87-4B67-88D4-269A39CA79E0}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Beer</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{EC4ADD68-C718-4DC5-8FA5-542E9E6128E1}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Coffee</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{7CF04FF4-7FFE-4CD6-9DD5-49DEE78CCE73}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Tea</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling max="75" min="45"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Hue</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Hue</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+          </a:endParaRPr>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -877,20 +1133,535 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -926,8 +1697,91 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2804160" y="2061210"/>
-              <a:ext cx="5516880" cy="3569970"/>
+              <a:off x="792480" y="1725930"/>
+              <a:ext cx="7871460" cy="5246370"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B6425E2-8FA3-F02B-1580-F17AF594D98B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2887980" y="1504950"/>
+              <a:ext cx="5234940" cy="3326130"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3006,6 +3860,1377 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FB2BFC-4ECD-4B3F-A97D-7486DB28395E}">
+  <dimension ref="A1:J103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>55.79</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>62.5</v>
+      </c>
+      <c r="D2">
+        <v>67.56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <f>MIN(A:A)</f>
+        <v>49.57</v>
+      </c>
+      <c r="H2">
+        <f>MIN(B:B)</f>
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <f>MIN(C:C)</f>
+        <v>60</v>
+      </c>
+      <c r="J2">
+        <f>MIN(D:D)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>55.79</v>
+      </c>
+      <c r="B3">
+        <v>60</v>
+      </c>
+      <c r="C3">
+        <v>66.55</v>
+      </c>
+      <c r="D3">
+        <v>67.09</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <f>_xlfn.QUARTILE.INC(A:A,1)</f>
+        <v>52.739999999999995</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:J3" si="0">_xlfn.QUARTILE.INC(B:B,1)</f>
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>62.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>56.13</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>68.16</v>
+      </c>
+      <c r="D4">
+        <v>65.67</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <f>_xlfn.QUARTILE.INC(A:A,2)</f>
+        <v>54.15</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:J4" si="1">_xlfn.QUARTILE.INC(B:B,2)</f>
+        <v>63.93</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>63.685000000000002</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>65.009999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>56.13</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <v>63.93</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <f>_xlfn.QUARTILE.INC(A:A,3)</f>
+        <v>55.18</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:J5" si="2">_xlfn.QUARTILE.INC(B:B,3)</f>
+        <v>66.324999999999989</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>65.0625</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>56.13</v>
+      </c>
+      <c r="B6">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <v>63.53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <f>MAX(A:A)</f>
+        <v>56.25</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:J6" si="3">MAX(B:B)</f>
+        <v>69.08</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>70.86</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>55.24</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>63.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>55.31</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8">
+        <v>63.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>55.38</v>
+      </c>
+      <c r="B9">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>63.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>56.25</v>
+      </c>
+      <c r="B10">
+        <v>68.97</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>63.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>55.24</v>
+      </c>
+      <c r="B11">
+        <v>68.64</v>
+      </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11">
+        <v>61.51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>56.13</v>
+      </c>
+      <c r="B12">
+        <v>63.27</v>
+      </c>
+      <c r="C12">
+        <v>60</v>
+      </c>
+      <c r="D12">
+        <v>63.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>63.82</v>
+      </c>
+      <c r="C13">
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>62.54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>55.56</v>
+      </c>
+      <c r="B14">
+        <v>63.3</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>55.71</v>
+      </c>
+      <c r="B15">
+        <v>64.290000000000006</v>
+      </c>
+      <c r="C15">
+        <v>60</v>
+      </c>
+      <c r="D15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>55.29</v>
+      </c>
+      <c r="B16">
+        <v>65.260000000000005</v>
+      </c>
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>61.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>49.57</v>
+      </c>
+      <c r="B17">
+        <v>67.12</v>
+      </c>
+      <c r="C17">
+        <v>65.78</v>
+      </c>
+      <c r="D17">
+        <v>62.54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>52.68</v>
+      </c>
+      <c r="B18">
+        <v>66.67</v>
+      </c>
+      <c r="C18">
+        <v>63.05</v>
+      </c>
+      <c r="D18">
+        <v>63.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>53.02</v>
+      </c>
+      <c r="B19">
+        <v>66.72</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>68.64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>53.02</v>
+      </c>
+      <c r="B20">
+        <v>65.790000000000006</v>
+      </c>
+      <c r="C20">
+        <v>61.44</v>
+      </c>
+      <c r="D20">
+        <v>64.319999999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>54.42</v>
+      </c>
+      <c r="B21">
+        <v>66.72</v>
+      </c>
+      <c r="C21">
+        <v>62.98</v>
+      </c>
+      <c r="D21">
+        <v>63.87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>53.48</v>
+      </c>
+      <c r="B22">
+        <v>65.36</v>
+      </c>
+      <c r="C22">
+        <v>62.86</v>
+      </c>
+      <c r="D22">
+        <v>63.31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>55.1</v>
+      </c>
+      <c r="B23">
+        <v>66.319999999999993</v>
+      </c>
+      <c r="C23">
+        <v>62.34</v>
+      </c>
+      <c r="D23">
+        <v>62.88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>55.2</v>
+      </c>
+      <c r="B24">
+        <v>65.22</v>
+      </c>
+      <c r="C24">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>64.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>55.86</v>
+      </c>
+      <c r="B25">
+        <v>65.69</v>
+      </c>
+      <c r="C25">
+        <v>60</v>
+      </c>
+      <c r="D25">
+        <v>63.36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>54.83</v>
+      </c>
+      <c r="B26">
+        <v>65.22</v>
+      </c>
+      <c r="C26">
+        <v>60</v>
+      </c>
+      <c r="D26">
+        <v>63.31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>55.08</v>
+      </c>
+      <c r="B27">
+        <v>66.209999999999994</v>
+      </c>
+      <c r="C27">
+        <v>60</v>
+      </c>
+      <c r="D27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>55.16</v>
+      </c>
+      <c r="B28">
+        <v>67</v>
+      </c>
+      <c r="C28">
+        <v>60</v>
+      </c>
+      <c r="D28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>55.16</v>
+      </c>
+      <c r="B29">
+        <v>68.5</v>
+      </c>
+      <c r="C29">
+        <v>60</v>
+      </c>
+      <c r="D29">
+        <v>65.81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>52.5</v>
+      </c>
+      <c r="B30">
+        <v>60</v>
+      </c>
+      <c r="C30">
+        <v>60</v>
+      </c>
+      <c r="D30">
+        <v>62.52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>52.8</v>
+      </c>
+      <c r="B31">
+        <v>60</v>
+      </c>
+      <c r="C31">
+        <v>60</v>
+      </c>
+      <c r="D31">
+        <v>63.81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>52.17</v>
+      </c>
+      <c r="B32">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>60</v>
+      </c>
+      <c r="D32">
+        <v>67.239999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>54.74</v>
+      </c>
+      <c r="B33">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>60</v>
+      </c>
+      <c r="D33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>54.92</v>
+      </c>
+      <c r="B34">
+        <v>60</v>
+      </c>
+      <c r="C34">
+        <v>60</v>
+      </c>
+      <c r="D34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>54.83</v>
+      </c>
+      <c r="B35">
+        <v>60</v>
+      </c>
+      <c r="C35">
+        <v>60</v>
+      </c>
+      <c r="D35">
+        <v>60.81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>54.83</v>
+      </c>
+      <c r="B36">
+        <v>62.48</v>
+      </c>
+      <c r="C36">
+        <v>60</v>
+      </c>
+      <c r="D36">
+        <v>62.78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>53.79</v>
+      </c>
+      <c r="B37">
+        <v>64.84</v>
+      </c>
+      <c r="C37">
+        <v>70.86</v>
+      </c>
+      <c r="D37">
+        <v>63.44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>54.92</v>
+      </c>
+      <c r="B38">
+        <v>66.290000000000006</v>
+      </c>
+      <c r="C38">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="D38">
+        <v>62.98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>55</v>
+      </c>
+      <c r="B39">
+        <v>62</v>
+      </c>
+      <c r="C39">
+        <v>65.41</v>
+      </c>
+      <c r="D39">
+        <v>63.47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>53.14</v>
+      </c>
+      <c r="B40">
+        <v>63.93</v>
+      </c>
+      <c r="C40">
+        <v>64.959999999999994</v>
+      </c>
+      <c r="D40">
+        <v>63.44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>54.15</v>
+      </c>
+      <c r="B41">
+        <v>63.93</v>
+      </c>
+      <c r="C41">
+        <v>65.5</v>
+      </c>
+      <c r="D41">
+        <v>63.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>54.15</v>
+      </c>
+      <c r="B42">
+        <v>62.98</v>
+      </c>
+      <c r="C42">
+        <v>65.45</v>
+      </c>
+      <c r="D42">
+        <v>64.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>53.02</v>
+      </c>
+      <c r="B43">
+        <v>69.08</v>
+      </c>
+      <c r="C43">
+        <v>65</v>
+      </c>
+      <c r="D43">
+        <v>64.349999999999994</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>55.1</v>
+      </c>
+      <c r="B44">
+        <v>69.08</v>
+      </c>
+      <c r="C44">
+        <v>65.040000000000006</v>
+      </c>
+      <c r="D44">
+        <v>65.709999999999994</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>53.75</v>
+      </c>
+      <c r="B45">
+        <v>60</v>
+      </c>
+      <c r="C45">
+        <v>66</v>
+      </c>
+      <c r="D45">
+        <v>66.34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>53.62</v>
+      </c>
+      <c r="B46">
+        <v>60</v>
+      </c>
+      <c r="C46">
+        <v>66.05</v>
+      </c>
+      <c r="D46">
+        <v>66.39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>53.75</v>
+      </c>
+      <c r="B47">
+        <v>60</v>
+      </c>
+      <c r="C47">
+        <v>66</v>
+      </c>
+      <c r="D47">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>53.75</v>
+      </c>
+      <c r="B48">
+        <v>60</v>
+      </c>
+      <c r="C48">
+        <v>66</v>
+      </c>
+      <c r="D48">
+        <v>66.61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>53.75</v>
+      </c>
+      <c r="B49">
+        <v>60</v>
+      </c>
+      <c r="C49">
+        <v>65.55</v>
+      </c>
+      <c r="D49">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>55</v>
+      </c>
+      <c r="B50">
+        <v>60.96</v>
+      </c>
+      <c r="C50">
+        <v>66.72</v>
+      </c>
+      <c r="D50">
+        <v>66.150000000000006</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>53.48</v>
+      </c>
+      <c r="B51">
+        <v>61.42</v>
+      </c>
+      <c r="C51">
+        <v>67.83</v>
+      </c>
+      <c r="D51">
+        <v>68.78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>53.48</v>
+      </c>
+      <c r="B52">
+        <v>61.42</v>
+      </c>
+      <c r="C52">
+        <v>60</v>
+      </c>
+      <c r="D52">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>53.62</v>
+      </c>
+      <c r="B53">
+        <v>61.88</v>
+      </c>
+      <c r="C53">
+        <v>65.36</v>
+      </c>
+      <c r="D53">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52.5</v>
+      </c>
+      <c r="B54">
+        <v>62.81</v>
+      </c>
+      <c r="C54">
+        <v>66.06</v>
+      </c>
+      <c r="D54">
+        <v>68.430000000000007</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53.62</v>
+      </c>
+      <c r="B55">
+        <v>63.33</v>
+      </c>
+      <c r="C55">
+        <v>65.66</v>
+      </c>
+      <c r="D55">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>51.52</v>
+      </c>
+      <c r="B56">
+        <v>63.31</v>
+      </c>
+      <c r="C56">
+        <v>65.56</v>
+      </c>
+      <c r="D56">
+        <v>67.06</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>51.96</v>
+      </c>
+      <c r="B57">
+        <v>62.86</v>
+      </c>
+      <c r="C57">
+        <v>62.83</v>
+      </c>
+      <c r="D57">
+        <v>66.61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>51.92</v>
+      </c>
+      <c r="B58">
+        <v>62.4</v>
+      </c>
+      <c r="C58">
+        <v>62.86</v>
+      </c>
+      <c r="D58">
+        <v>67.12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>51.92</v>
+      </c>
+      <c r="B59">
+        <v>64.22</v>
+      </c>
+      <c r="C59">
+        <v>62.86</v>
+      </c>
+      <c r="D59">
+        <v>66.61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>51.92</v>
+      </c>
+      <c r="B60">
+        <v>61.94</v>
+      </c>
+      <c r="C60">
+        <v>63.89</v>
+      </c>
+      <c r="D60">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>51.92</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <v>63.89</v>
+      </c>
+      <c r="D61">
+        <v>64.290000000000006</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>51.09</v>
+      </c>
+      <c r="B62">
+        <v>60</v>
+      </c>
+      <c r="C62">
+        <v>64.290000000000006</v>
+      </c>
+      <c r="D62">
+        <v>62.68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>51.68</v>
+      </c>
+      <c r="B63">
+        <v>60</v>
+      </c>
+      <c r="C63">
+        <v>64.36</v>
+      </c>
+      <c r="D63">
+        <v>62.65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>51.33</v>
+      </c>
+      <c r="B64">
+        <v>60</v>
+      </c>
+      <c r="C64">
+        <v>63.85</v>
+      </c>
+      <c r="D64">
+        <v>60.53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>50.23</v>
+      </c>
+      <c r="B65">
+        <v>60</v>
+      </c>
+      <c r="C65">
+        <v>64.819999999999993</v>
+      </c>
+      <c r="D65">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>50.34</v>
+      </c>
+      <c r="B66">
+        <v>66.77</v>
+      </c>
+      <c r="C66">
+        <v>64.36</v>
+      </c>
+      <c r="D66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>52.6</v>
+      </c>
+      <c r="B67">
+        <v>64.92</v>
+      </c>
+      <c r="C67">
+        <v>63.85</v>
+      </c>
+      <c r="D67">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>55.86</v>
+      </c>
+      <c r="B68">
+        <v>64</v>
+      </c>
+      <c r="C68">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D68">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>63.53</v>
+      </c>
+      <c r="C69">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="D69">
+        <v>62.98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>64</v>
+      </c>
+      <c r="C70">
+        <v>64.36</v>
+      </c>
+      <c r="D70">
+        <v>62.98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>64</v>
+      </c>
+      <c r="C71">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="D71">
+        <v>62.46</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>64.459999999999994</v>
+      </c>
+      <c r="C72">
+        <v>63.65</v>
+      </c>
+      <c r="D72">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>64.92</v>
+      </c>
+      <c r="C73">
+        <v>65.13</v>
+      </c>
+      <c r="D73">
+        <v>62.48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>64.459999999999994</v>
+      </c>
+      <c r="C74">
+        <v>63.65</v>
+      </c>
+      <c r="D74">
+        <v>66.77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>65.41</v>
+      </c>
+      <c r="C75">
+        <v>63.62</v>
+      </c>
+      <c r="D75">
+        <v>66.290000000000006</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>66.34</v>
+      </c>
+      <c r="C76">
+        <v>65.13</v>
+      </c>
+      <c r="D76">
+        <v>65.849999999999994</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>66.34</v>
+      </c>
+      <c r="C77">
+        <v>64.66</v>
+      </c>
+      <c r="D77">
+        <v>66.83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>67.260000000000005</v>
+      </c>
+      <c r="C78">
+        <v>64.7</v>
+      </c>
+      <c r="D78">
+        <v>66.39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="C79">
+        <v>64.17</v>
+      </c>
+      <c r="D79">
+        <v>65.22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="C80">
+        <v>64.209999999999994</v>
+      </c>
+      <c r="D80">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>68.5</v>
+      </c>
+      <c r="C81">
+        <v>63.72</v>
+      </c>
+      <c r="D81">
+        <v>61.88</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>68.5</v>
+      </c>
+      <c r="C82">
+        <v>63.72</v>
+      </c>
+      <c r="D82">
+        <v>65.33</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>68.03</v>
+      </c>
+      <c r="C83">
+        <v>62.7</v>
+      </c>
+      <c r="D83">
+        <v>65.45</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>67.14</v>
+      </c>
+      <c r="C84">
+        <v>61.64</v>
+      </c>
+      <c r="D84">
+        <v>66.55</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>66.34</v>
+      </c>
+      <c r="C85">
+        <v>62.16</v>
+      </c>
+      <c r="D85">
+        <v>65.790000000000006</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <v>61.64</v>
+      </c>
+      <c r="D86">
+        <v>66.260000000000005</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <v>61.64</v>
+      </c>
+      <c r="D87">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <v>65.64</v>
+      </c>
+      <c r="D88">
+        <v>67.87</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <v>65.17</v>
+      </c>
+      <c r="D89">
+        <v>66.72</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>67.12</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <v>69.84</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D96">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D98">
+        <v>67.06</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <v>67.12</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <v>63.93</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D102">
+        <v>65.790000000000006</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <v>66.37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FE4E8A-C6C5-4B53-ADDC-E2A2BE85FED8}">
   <dimension ref="A1:W26"/>
@@ -5523,8 +7748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DFCF4A-567D-4CC8-B150-F76E428A5D5A}">
   <dimension ref="A1:AC42"/>
   <sheetViews>
-    <sheetView topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2:AB32"/>
+    <sheetView topLeftCell="Q2" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7749,8 +9974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719D8396-4F96-4D3C-9AD7-FE3B47BA4C06}">
   <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9339,7 +11564,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9347,8 +11573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2182987-33A6-4FED-91C7-45E7131A1B14}">
   <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2:AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10490,8 +12716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B1B2B3-2F65-4636-B2E0-97CC1247D88C}">
   <dimension ref="A1:AC24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:L1"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2:AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11900,8 +14126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DD5A72-5FA6-4114-970B-4F083341F838}">
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2:AB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13364,8 +15590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5B6B2-ABCA-43DE-A2A7-6E2A5A8925B1}">
   <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2:AB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>